<commit_message>
completed o__bacillales, o__Erysipelotrichales, o__Lactobacillales, o__mycoplasmatales, o__RFN20
</commit_message>
<xml_diff>
--- a/outputs/o__Erysipelotrichales.xlsx
+++ b/outputs/o__Erysipelotrichales.xlsx
@@ -1,61 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="o__Erysipelotrichales_pred-t" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="o__Erysipelotrichales_pred-t" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="o__Erysipelotrichales_pred-t-p" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
-  <si>
-    <t>f__Erysipelatoclostridiaceae-f__Erysipelotrichaceae</t>
-  </si>
-  <si>
-    <t>prediction</t>
-  </si>
-  <si>
-    <t>RUG293</t>
-  </si>
-  <si>
-    <t>f__Erysipelatoclostridiaceae</t>
-  </si>
-  <si>
-    <t>RUG287</t>
-  </si>
-  <si>
-    <t>RUG016</t>
-  </si>
-  <si>
-    <t>f__Erysipelotrichaceae</t>
-  </si>
-  <si>
-    <t>RUG017</t>
-  </si>
-  <si>
-    <t>RUG262</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -69,12 +43,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -86,18 +75,89 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -392,76 +452,311 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae-f__Erysipelotrichaceae</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>prediction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>RUG293</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-1.308411839796172</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>RUG287</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-0.3631716122027165</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>RUG016</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.2592044217448454</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>f__Erysipelotrichaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>RUG017</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.08107671139596583</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>RUG262</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.06961040564839381</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>f__Erysipelotrichaceae</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MAG</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>f__Erysipelotrichaceae</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>prediction</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>rejection-f</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>gtdb-Tk</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>RUG293</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.308411839796172</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>0.7872472778589438</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.2127527221410562</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.7872472778589438</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>f__CAG-313</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>RUG287</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.3631716122027165</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>0.5898079745388198</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.4101920254611801</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.5898079745388198</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>RUG016</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2592044217448454</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>0.435559289001053</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.564440710998947</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.564440710998947</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>f__Erysipelotrichaceae</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RUG017</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.08107671139596583</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>0.5202580819689697</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.4797419180310303</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.5202580819689697</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>RUG262</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06961040564839381</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
+        <v>0.4826044223673577</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5173955776326423</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5173955776326423</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>f__Erysipelotrichaceae</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>f__Erysipelatoclostridiaceae</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>